<commit_message>
Structure changes, improve documentation.
</commit_message>
<xml_diff>
--- a/domain_files/ifdat/example/BSI_MFMC_M0_EXAMPLE.xlsx
+++ b/domain_files/ifdat/example/BSI_MFMC_M0_EXAMPLE.xlsx
@@ -686,7 +686,7 @@
     <row r="3" ht="40" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>SOURCE_ORG</t>
+          <t>DOMAIN</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -698,7 +698,7 @@
     <row r="4" ht="40" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>SOURCE_PERSON</t>
+          <t>CATEGORY</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -710,26 +710,18 @@
     <row r="5" ht="40" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>CATEGORY</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>IFDAT</t>
-        </is>
-      </c>
+          <t>SOURCE_ORG</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr"/>
     </row>
     <row r="6" ht="40" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>SUB_CATEGORY</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>BSI</t>
-        </is>
-      </c>
+          <t>SOURCE_PERSON</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -742,7 +734,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -753,7 +745,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -770,7 +762,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -787,7 +779,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -799,7 +791,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -811,208 +803,215 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -1972,7 +1971,7 @@
   </mergeCells>
   <dataValidations count="17">
     <dataValidation sqref="D4:D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'SHARE_'!$A$1:$A$34</formula1>
+      <formula1>'SHARE_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20 W4:W20 Y4:Y20 AA4:AA20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'SHARE_'!$B$1:$B$4</formula1>
@@ -2036,7 +2035,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2047,7 +2046,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -2064,7 +2063,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2081,7 +2080,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2093,7 +2092,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2105,208 +2104,215 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -3058,10 +3064,10 @@
   </mergeCells>
   <dataValidations count="14">
     <dataValidation sqref="D4:D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'EXT_DERIVATIVE_'!$A$1:$A$34</formula1>
+      <formula1>'EXT_DERIVATIVE_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'EXT_DERIVATIVE_'!$B$1:$B$4</formula1>
+      <formula1>'EXT_DERIVATIVE_'!$B$1:$B$5</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'EXT_DERIVATIVE_'!$C$1:$C$4</formula1>
@@ -3113,7 +3119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3124,12 +3130,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>MICRO_HEDGE</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -3146,12 +3152,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MACRO_HEDGE</t>
+          <t>MICRO_HEDGE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3168,12 +3174,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PORT_MGMNT</t>
+          <t>MACRO_HEDGE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3185,12 +3191,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SPECULATIVE</t>
+          <t>PORT_MGMNT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3202,208 +3208,220 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SPECULATIVE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -3949,10 +3967,10 @@
   </mergeCells>
   <dataValidations count="10">
     <dataValidation sqref="C4:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'OTC_DERIVATIVE_'!$A$1:$A$34</formula1>
+      <formula1>'OTC_DERIVATIVE_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="G4:G20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'OTC_DERIVATIVE_'!$B$1:$B$4</formula1>
+      <formula1>'OTC_DERIVATIVE_'!$B$1:$B$5</formula1>
     </dataValidation>
     <dataValidation sqref="H4:H20 J4:J20 L4:L20 N4:N20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'OTC_DERIVATIVE_'!$C$1:$C$4</formula1>
@@ -3992,7 +4010,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4003,12 +4021,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>MICRO_HEDGE</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -4025,12 +4043,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MACRO_HEDGE</t>
+          <t>MICRO_HEDGE</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -4047,12 +4065,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PORT_MGMNT</t>
+          <t>MACRO_HEDGE</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -4064,12 +4082,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SPECULATIVE</t>
+          <t>PORT_MGMNT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -4081,208 +4099,220 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SPECULATIVE</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -5006,7 +5036,7 @@
   </mergeCells>
   <dataValidations count="13">
     <dataValidation sqref="C4:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'RESIDENTIAL_RE_'!$A$1:$A$34</formula1>
+      <formula1>'RESIDENTIAL_RE_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'RESIDENTIAL_RE_'!$B$1:$B$4</formula1>
@@ -5058,7 +5088,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5069,7 +5099,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -5086,7 +5116,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -5103,7 +5133,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -5115,7 +5145,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -5127,208 +5157,215 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -6052,7 +6089,7 @@
   </mergeCells>
   <dataValidations count="13">
     <dataValidation sqref="C4:C20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'COMMERCIAL_RE_'!$A$1:$A$34</formula1>
+      <formula1>'COMMERCIAL_RE_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20 T4:T20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'COMMERCIAL_RE_'!$B$1:$B$4</formula1>
@@ -6301,7 +6338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6312,7 +6349,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -6329,7 +6366,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6346,7 +6383,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -6358,7 +6395,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -6370,208 +6407,215 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -7351,13 +7395,13 @@
   </mergeCells>
   <dataValidations count="15">
     <dataValidation sqref="A4:A20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'REM_FIXED_'!$A$1:$A$13</formula1>
+      <formula1>'REM_FIXED_'!$A$1:$A$14</formula1>
     </dataValidation>
     <dataValidation sqref="B4:B20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'REM_FIXED_'!$B$1:$B$103</formula1>
     </dataValidation>
     <dataValidation sqref="E4:E20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'REM_FIXED_'!$C$1:$C$34</formula1>
+      <formula1>'REM_FIXED_'!$C$1:$C$35</formula1>
     </dataValidation>
     <dataValidation sqref="L4:L20 N4:N20 P4:P20 R4:R20 T4:T20 V4:V20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'REM_FIXED_'!$D$1:$D$4</formula1>
@@ -7420,7 +7464,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>N1131</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -7430,7 +7474,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -7447,7 +7491,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>N1132</t>
+          <t>N1131</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -7457,7 +7501,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -7474,7 +7518,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>N1139</t>
+          <t>N1132</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -7484,7 +7528,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -7496,7 +7540,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>N114</t>
+          <t>N1139</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -7506,7 +7550,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -7518,7 +7562,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>N115</t>
+          <t>N114</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7528,14 +7572,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N1171</t>
+          <t>N115</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -7545,14 +7589,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>N1172</t>
+          <t>N1171</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -7562,14 +7606,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N1173</t>
+          <t>N1172</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -7579,14 +7623,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>N1174</t>
+          <t>N1173</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7596,14 +7640,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>N1179</t>
+          <t>N1174</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -7613,14 +7657,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>N131</t>
+          <t>N1179</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -7630,14 +7674,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>N132</t>
+          <t>N131</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -7647,36 +7691,41 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>N132</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>N133</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>BR</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BS</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>A5</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>BS</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>A10</t>
         </is>
       </c>
     </row>
@@ -7688,7 +7737,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
@@ -7700,7 +7749,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
@@ -7712,7 +7761,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
@@ -7724,7 +7773,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
@@ -7736,7 +7785,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
@@ -7748,7 +7797,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
@@ -7760,7 +7809,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
@@ -7772,7 +7821,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
@@ -7784,7 +7833,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
@@ -7796,7 +7845,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
@@ -7808,7 +7857,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
@@ -7820,7 +7869,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
@@ -7832,7 +7881,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
@@ -7844,7 +7893,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
@@ -7856,7 +7905,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
@@ -7868,7 +7917,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -7880,7 +7929,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
@@ -7892,7 +7941,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
@@ -7904,7 +7953,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
@@ -7916,7 +7965,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>_Z</t>
+          <t>_U</t>
         </is>
       </c>
     </row>
@@ -7924,6 +7973,11 @@
       <c r="B35" t="inlineStr">
         <is>
           <t>FR</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>_Z</t>
         </is>
       </c>
     </row>
@@ -21754,7 +21808,7 @@
   </mergeCells>
   <dataValidations count="13">
     <dataValidation sqref="D4:D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'LIAB_DEBT_'!$A$1:$A$34</formula1>
+      <formula1>'LIAB_DEBT_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="K4:K20 M4:M20 O4:O20 Q4:Q20 S4:S20 U4:U20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'LIAB_DEBT_'!$B$1:$B$4</formula1>
@@ -21806,7 +21860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21817,7 +21871,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -21834,7 +21888,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -21851,7 +21905,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -21863,7 +21917,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -21875,208 +21929,215 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -36193,7 +36254,7 @@
   </mergeCells>
   <dataValidations count="11">
     <dataValidation sqref="D4:D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'HOLDER_'!$A$1:$A$34</formula1>
+      <formula1>'HOLDER_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="J4:J20 L4:L20 N4:N20 P4:P20 R4:R20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'HOLDER_'!$B$1:$B$4</formula1>
@@ -36239,7 +36300,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36250,7 +36311,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -36267,7 +36328,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -36284,7 +36345,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -36296,7 +36357,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -36308,208 +36369,215 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>N</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>Q</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>S</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>W</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A10</t>
+          <t>A5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>A20</t>
+          <t>A10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A30</t>
+          <t>A20</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>A_3</t>
+          <t>A30</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>M2</t>
+          <t>A_3</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>M_2</t>
+          <t>M2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>M_3</t>
+          <t>M_2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>W2</t>
+          <t>M_3</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>W3</t>
+          <t>W2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>W4</t>
+          <t>W3</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>W_2</t>
+          <t>W4</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>W_3</t>
+          <t>W_2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D_2</t>
+          <t>W_3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>H2</t>
+          <t>D_2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>H3</t>
+          <t>H2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>H3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>OA</t>
+          <t>I</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>OA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>_O</t>
+          <t>OM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>_U</t>
+          <t>_O</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
+        <is>
+          <t>_U</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>_Z</t>
         </is>
@@ -39098,7 +39166,7 @@
   </mergeCells>
   <dataValidations count="21">
     <dataValidation sqref="D4:D20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>'ASSET_DEBT_'!$A$1:$A$34</formula1>
+      <formula1>'ASSET_DEBT_'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation sqref="O4:O20 Q4:Q20 S4:S20 U4:U20 W4:W20 Y4:Y20 AA4:AA20 AC4:AC20 AE4:AE20 AG4:AG20" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>'ASSET_DEBT_'!$B$1:$B$4</formula1>

</xml_diff>